<commit_message>
Tests: automate testing of database functions.
</commit_message>
<xml_diff>
--- a/samples/excel12/database.xlsx
+++ b/samples/excel12/database.xlsx
@@ -4,14 +4,17 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="6230"/>
+    <workbookView activeTab="1" windowWidth="14400" windowHeight="6230"/>
   </bookViews>
   <sheets>
-    <sheet name="Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Types" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Types"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Overview"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Types"</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
@@ -21,6 +24,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16" count="16">
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
     <t>Selector</t>
   </si>
   <si>
@@ -33,15 +45,9 @@
     <t>Field</t>
   </si>
   <si>
-    <t>&gt;=1</t>
-  </si>
-  <si>
     <t>DAVERAGE</t>
   </si>
   <si>
-    <t>Strict</t>
-  </si>
-  <si>
     <t>DMIN</t>
   </si>
   <si>
@@ -64,15 +70,15 @@
   </si>
   <si>
     <t>DVARP</t>
-  </si>
-  <si>
-    <t>Only numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="[&lt;=0]0;[Red]0" numFmtId="100"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <b val="0"/>
@@ -136,8 +142,17 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -158,7 +173,58 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>Types!B1</f>
+        <v>22</v>
+      </c>
+      <c r="C2" s="3">
+        <f>Types!B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15"/>
+    <row r="6" spans="1:3" ht="15"/>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
+  <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -171,116 +237,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Pass:</t>
         </is>
       </c>
       <c r="B1">
         <f t="array" ref="B1">SUM(0+D$18:D$10002)</f>
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Fail:</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <f t="array" ref="B2">SUM(0+ISLOGICAL(D$18:D$10028))-B1</f>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Float</t>
         </is>
       </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Error</t>
         </is>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="e">
+      <c r="C8" s="6" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Boolean</t>
         </is>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="b">
+      <c r="C9" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Blank</t>
         </is>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="15"/>
     <row r="13" spans="1:5">
@@ -296,26 +362,28 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>&gt;=1</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
         <is>
           <t>&lt;&gt;4</t>
         </is>
@@ -405,11 +473,11 @@
     </row>
     <row r="24" spans="1:5" ht="15">
       <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="e">
         <f>DAVERAGE($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C24" t="e">
         <f>SUM(C5:C10)</f>
@@ -417,19 +485,21 @@
       </c>
       <c r="D24" t="b">
         <f>IFERROR(ERROR.TYPE(B24)=ERROR.TYPE(C24),IFERROR(B24=C24,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Strict</t>
+        </is>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="e">
         <f>DMIN($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C25" t="e">
         <f>C24</f>
@@ -437,16 +507,16 @@
       </c>
       <c r="D25" t="b">
         <f>IFERROR(ERROR.TYPE(B25)=ERROR.TYPE(C25),IFERROR(B25=C25,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="e">
         <f>DMAX($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C26" t="e">
         <f>C25</f>
@@ -454,16 +524,16 @@
       </c>
       <c r="D26" t="b">
         <f>IFERROR(ERROR.TYPE(B26)=ERROR.TYPE(C26),IFERROR(B26=C26,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15">
       <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="e">
         <f>DPRODUCT($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C27" t="e">
         <f>C26</f>
@@ -471,16 +541,16 @@
       </c>
       <c r="D27" t="b">
         <f>IFERROR(ERROR.TYPE(B27)=ERROR.TYPE(C27),IFERROR(B27=C27,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15">
       <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="B28" t="e">
         <f>DSTDEV($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C28" t="e">
         <f>C27</f>
@@ -488,16 +558,16 @@
       </c>
       <c r="D28" t="b">
         <f>IFERROR(ERROR.TYPE(B28)=ERROR.TYPE(C28),IFERROR(B28=C28,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15">
       <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="B29" t="e">
         <f>DSTDEVP($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>0.81649658092772603</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C29" t="e">
         <f>C28</f>
@@ -505,16 +575,16 @@
       </c>
       <c r="D29" t="b">
         <f>IFERROR(ERROR.TYPE(B29)=ERROR.TYPE(C29),IFERROR(B29=C29,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15">
       <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="B30" t="e">
         <f>DSUM($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C30" t="e">
         <f>C29</f>
@@ -522,16 +592,16 @@
       </c>
       <c r="D30" t="b">
         <f>IFERROR(ERROR.TYPE(B30)=ERROR.TYPE(C30),IFERROR(B30=C30,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15">
       <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="e">
         <f>DVAR($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C31" t="e">
         <f>C30</f>
@@ -539,16 +609,16 @@
       </c>
       <c r="D31" t="b">
         <f>IFERROR(ERROR.TYPE(B31)=ERROR.TYPE(C31),IFERROR(B31=C31,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15">
       <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="e">
         <f>DVARP($A$4:$C$10,"Value",$A$15:$A$16)</f>
-        <v>0.66666666666666663</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C32" t="e">
         <f>C31</f>
@@ -556,13 +626,13 @@
       </c>
       <c r="D32" t="b">
         <f>IFERROR(ERROR.TYPE(B32)=ERROR.TYPE(C32),IFERROR(B32=C32,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15"/>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B35">
         <f>DAVERAGE($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -575,13 +645,15 @@
         <f>IFERROR(ERROR.TYPE(B35)=ERROR.TYPE(C35),IFERROR(B35=C35,FALSE))</f>
         <v>1</v>
       </c>
-      <c r="E35" t="s">
-        <v>15</v>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Only numbers</t>
+        </is>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <f>DMIN($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -597,7 +669,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37">
         <f>DMAX($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -613,7 +685,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <f>DPRODUCT($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -629,7 +701,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <f>DSTDEV($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -646,7 +718,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40">
         <f>DSTDEVP($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -663,7 +735,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <f>DSUM($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -679,7 +751,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B42">
         <f>DVAR($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -696,7 +768,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <f>DVARP($A$4:$C$10,"Value",$C$15:$C$16)</f>

</xml_diff>

<commit_message>
Tests: add tests for database function operators.
We currently fail.
</commit_message>
<xml_diff>
--- a/samples/excel12/database.xlsx
+++ b/samples/excel12/database.xlsx
@@ -4,17 +4,20 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1" windowWidth="14400" windowHeight="6230"/>
+    <workbookView activeTab="0" windowWidth="14400" windowHeight="6230"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Types" sheetId="2" r:id="rId2"/>
+    <sheet name="Operators" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Overview"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Types"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Operators"</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
@@ -22,17 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16" count="16">
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="22">
   <si>
     <t>Types</t>
   </si>
   <si>
+    <t>Operators</t>
+  </si>
+  <si>
+    <t>Pass:</t>
+  </si>
+  <si>
+    <t>Fail:</t>
+  </si>
+  <si>
     <t>Selector</t>
   </si>
   <si>
@@ -42,9 +48,18 @@
     <t>String</t>
   </si>
   <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
     <t>Field</t>
   </si>
   <si>
+    <t>&lt;&gt;4</t>
+  </si>
+  <si>
     <t>DAVERAGE</t>
   </si>
   <si>
@@ -70,6 +85,12 @@
   </si>
   <si>
     <t>DVARP</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Regexp</t>
   </si>
 </sst>
 </file>
@@ -175,26 +196,31 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="3" style="0" width="15.999038461538463" customWidth="1"/>
+    <col min="4" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <f>Types!B1</f>
@@ -203,6 +229,19 @@
       <c r="C2" s="3">
         <f>Types!B2</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>Operators!B1</f>
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <f>Operators!B2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15"/>
@@ -226,8 +265,8 @@
   </sheetPr>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -237,10 +276,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Pass:</t>
-        </is>
+      <c r="A1" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B1">
         <f t="array" ref="B1">SUM(0+D$18:D$10002)</f>
@@ -248,10 +285,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Fail:</t>
-        </is>
+      <c r="A2" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <f t="array" ref="B2">SUM(0+ISLOGICAL(D$18:D$10028))-B1</f>
@@ -265,10 +300,10 @@
         </is>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
@@ -299,7 +334,7 @@
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -325,10 +360,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
+      <c r="A9" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>5</v>
@@ -338,10 +371,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>Blank</t>
-        </is>
+      <c r="A10" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>6</v>
@@ -363,18 +394,18 @@
     </row>
     <row r="14" spans="1:5" ht="15">
       <c r="A14" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
       <c r="A15" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
@@ -383,10 +414,8 @@
           <t>&gt;=1</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
-        <is>
-          <t>&lt;&gt;4</t>
-        </is>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15">
@@ -473,7 +502,7 @@
     </row>
     <row r="24" spans="1:5" ht="15">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B24" t="e">
         <f>DAVERAGE($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -495,7 +524,7 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B25" t="e">
         <f>DMIN($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -512,7 +541,7 @@
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B26" t="e">
         <f>DMAX($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -529,7 +558,7 @@
     </row>
     <row r="27" spans="1:5" ht="15">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B27" t="e">
         <f>DPRODUCT($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -546,7 +575,7 @@
     </row>
     <row r="28" spans="1:5" ht="15">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B28" t="e">
         <f>DSTDEV($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -563,7 +592,7 @@
     </row>
     <row r="29" spans="1:5" ht="15">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B29" t="e">
         <f>DSTDEVP($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -580,7 +609,7 @@
     </row>
     <row r="30" spans="1:5" ht="15">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B30" t="e">
         <f>DSUM($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -597,7 +626,7 @@
     </row>
     <row r="31" spans="1:5" ht="15">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B31" t="e">
         <f>DVAR($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -614,7 +643,7 @@
     </row>
     <row r="32" spans="1:5" ht="15">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B32" t="e">
         <f>DVARP($A$4:$C$10,"Value",$A$15:$A$16)</f>
@@ -632,7 +661,7 @@
     <row r="33" spans="1:5" ht="15"/>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <f>DAVERAGE($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -653,7 +682,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B36">
         <f>DMIN($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -669,7 +698,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B37">
         <f>DMAX($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -685,7 +714,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B38">
         <f>DPRODUCT($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -701,7 +730,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B39">
         <f>DSTDEV($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -718,7 +747,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B40">
         <f>DSTDEVP($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -735,7 +764,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <f>DSUM($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -751,7 +780,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <f>DVAR($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -768,7 +797,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B43">
         <f>DVARP($A$4:$C$10,"Value",$C$15:$C$16)</f>
@@ -781,6 +810,654 @@
       <c r="D43" t="b">
         <f>IFERROR(ERROR.TYPE(B43)=ERROR.TYPE(C43),IFERROR(B43=C43,FALSE))</f>
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
+  <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" style="0" width="16.427584134615387" customWidth="1"/>
+    <col min="3" max="16384" style="0" width="9.142307692307693"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <f t="array" ref="B1">SUM(0+E$24:E$10000)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <f t="array" ref="B2">SUM(0+ISLOGICAL(E$24:E$10000))-B1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15">
+      <c r="A13" s="6">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="6">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15">
+      <c r="A24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <f>DSUM($A$4:$B$19,"Value",A25:A26)</f>
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24" t="b">
+        <f>C24=D24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15">
+      <c r="A25" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>=4</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15">
+      <c r="A28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <f>DSUM($A$4:$B$19,"Value",A29:A30)</f>
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28" t="b">
+        <f>C28=D28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>&lt;4</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15">
+      <c r="A32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <f>DSUM($A$4:$B$19,"Value",A33:A34)</f>
+        <v>2016</v>
+      </c>
+      <c r="D32">
+        <v>2016</v>
+      </c>
+      <c r="E32" t="b">
+        <f>C32=D32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>&gt;4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15">
+      <c r="A36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <f>DSUM($A$4:$B$19,"Value",A37:A38)</f>
+        <v>31</v>
+      </c>
+      <c r="D36">
+        <v>31</v>
+      </c>
+      <c r="E36" t="b">
+        <f>C36=D36</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15">
+      <c r="A37" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>&lt;=4</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15">
+      <c r="A40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <f>DSUM($A$4:$B$19,"Value",A41:A42)</f>
+        <v>2032</v>
+      </c>
+      <c r="D40">
+        <v>2032</v>
+      </c>
+      <c r="E40" t="b">
+        <f>C40=D40</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15">
+      <c r="A41" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>&gt;=4</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15">
+      <c r="A44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <f>DSUM($A$4:$B$19,"Value",A45:A46)</f>
+        <v>2031</v>
+      </c>
+      <c r="D44">
+        <v>2031</v>
+      </c>
+      <c r="E44" t="b">
+        <f>C44=D44</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15">
+      <c r="A45" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15">
+      <c r="A46" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15">
+      <c r="A48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <f>DSUM($A$4:$B$19,"Value",A49:A50)</f>
+        <v>1026</v>
+      </c>
+      <c r="D48">
+        <v>1026</v>
+      </c>
+      <c r="E48" t="b">
+        <f>C48=D48</f>
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15">
+      <c r="A49" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>1*</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15">
+      <c r="A52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <f>DSUM($A$4:$B$19,"Value",A53:A54)</f>
+        <v>1023</v>
+      </c>
+      <c r="D52">
+        <v>1023</v>
+      </c>
+      <c r="E52" t="b">
+        <f>C52=D52</f>
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15">
+      <c r="A53" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15">
+      <c r="A54" s="6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15">
+      <c r="A56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <f>DSUM($A$4:$B$19,"Value",A57:A58)</f>
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2048</v>
+      </c>
+      <c r="E56" t="b">
+        <f>C56=D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15">
+      <c r="A57" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15">
+      <c r="A58" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15">
+      <c r="A60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <f>DSUM($A$4:$B$19,"Value",A61:A62)</f>
+        <v>30719</v>
+      </c>
+      <c r="D60">
+        <f>2^15-1-2048</f>
+        <v>30719</v>
+      </c>
+      <c r="E60" t="b">
+        <f>C60=D60</f>
+        <v>1</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Nonblank</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15">
+      <c r="A61" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15">
+      <c r="A62" s="6" t="inlineStr">
+        <is>
+          <t>&lt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15">
+      <c r="A64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <f>DSUM($A$4:$B$19,"Value",A65:A66)</f>
+        <v>64</v>
+      </c>
+      <c r="D64">
+        <v>64</v>
+      </c>
+      <c r="E64" t="b">
+        <f>C64=D64</f>
+        <v>1</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15">
+      <c r="A65" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15">
+      <c r="A66" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15">
+      <c r="A68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <f>DSUM($A$4:$B$19,"Value",A69:A70)</f>
+        <v>8192</v>
+      </c>
+      <c r="D68">
+        <v>8192</v>
+      </c>
+      <c r="E68" t="b">
+        <f>C68=D68</f>
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15">
+      <c r="A69" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15">
+      <c r="A72" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72">
+        <f>DSUM($A$4:$B$19,"Value",A73:A74)</f>
+        <v>4096</v>
+      </c>
+      <c r="D72">
+        <v>4096</v>
+      </c>
+      <c r="E72" t="b">
+        <f>C72=D72</f>
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15">
+      <c r="A73" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15">
+      <c r="A76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <f>DSUM($A$4:$B$19,"Value",A77:A78)</f>
+        <v>8192</v>
+      </c>
+      <c r="D76">
+        <v>8192</v>
+      </c>
+      <c r="E76" t="b">
+        <f>C76=D76</f>
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Boolean as string</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15">
+      <c r="A77" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15">
+      <c r="A78" s="6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15">
+      <c r="A80" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80">
+        <f>DSUM($A$4:$B$19,"Value",A81:A82)</f>
+        <v>16384</v>
+      </c>
+      <c r="D80">
+        <v>16384</v>
+      </c>
+      <c r="E80" t="b">
+        <f>C80=D80</f>
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15">
+      <c r="A81" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15">
+      <c r="A82" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15">
+      <c r="A84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <f>DSUM($A$4:$B$19,"Value",A85:A86)</f>
+        <v>16384</v>
+      </c>
+      <c r="D84">
+        <v>16384</v>
+      </c>
+      <c r="E84" t="b">
+        <f>C84=D84</f>
+        <v>1</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Regexp, different case</t>
+        </is>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15">
+      <c r="A85" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15">
+      <c r="A86" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
D-funcs: fix handling of blanks.
Also update expected values.  We still fail.
</commit_message>
<xml_diff>
--- a/samples/excel12/database.xlsx
+++ b/samples/excel12/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="6230"/>
+    <workbookView activeTab="2" windowWidth="14400" windowHeight="6230"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
     <t>string</t>
   </si>
   <si>
-    <t>Regexp</t>
+    <t>Regexps only match strings</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -237,11 +237,11 @@
       </c>
       <c r="B3">
         <f>Operators!B1</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <f>Operators!B2</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15"/>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="B1">
         <f t="array" ref="B1">SUM(0+E$24:E$10000)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
@@ -856,7 +856,7 @@
       </c>
       <c r="B2" s="3">
         <f t="array" ref="B2">SUM(0+ISLOGICAL(E$24:E$10000))-B1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15">
@@ -1130,15 +1130,14 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <f>DSUM($A$4:$B$19,"Value",A45:A46)</f>
-        <v>2031</v>
+        <v>32751</v>
       </c>
       <c r="D44">
         <v>2031</v>
       </c>
       <c r="E44" t="b">
         <f>C44=D44</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15">
@@ -1156,15 +1155,14 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <f>DSUM($A$4:$B$19,"Value",A49:A50)</f>
-        <v>1026</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>1026</v>
       </c>
       <c r="E48" t="b">
         <f>C48=D48</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="s">
         <v>21</v>
@@ -1187,15 +1185,14 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <f>DSUM($A$4:$B$19,"Value",A53:A54)</f>
-        <v>1023</v>
+        <v>16384</v>
       </c>
       <c r="D52">
         <v>1023</v>
       </c>
       <c r="E52" t="b">
         <f>C52=D52</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
         <v>21</v>
@@ -1219,14 +1216,14 @@
       </c>
       <c r="C56">
         <f>DSUM($A$4:$B$19,"Value",A57:A58)</f>
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="D56">
         <v>2048</v>
       </c>
       <c r="E56" t="b">
         <f>C56=D56</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
@@ -1415,8 +1412,10 @@
         <f>C80=D80</f>
         <v>1</v>
       </c>
-      <c r="F80" t="s">
-        <v>21</v>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Regexp</t>
+        </is>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15">

</xml_diff>

<commit_message>
Tests: more tests for regexp matching in F-funcs
</commit_message>
<xml_diff>
--- a/samples/excel12/database.xlsx
+++ b/samples/excel12/database.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29" count="29">
   <si>
     <t>Types</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Regexps only match strings</t>
+  </si>
+  <si>
+    <t>Regexp</t>
+  </si>
+  <si>
+    <t>=string</t>
+  </si>
+  <si>
+    <t>str</t>
   </si>
   <si>
     <t>Selector1</t>
@@ -170,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="9">
     <border diagonalUp="0" diagonalDown="0">
       <start style="none">
         <color rgb="FFC7C7C7"/>
@@ -183,90 +192,6 @@
       </top>
       <bottom style="none">
         <color rgb="FFC7C7C7"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="thin">
-        <color rgb="FF000000"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="thin">
-        <color rgb="FF000000"/>
-      </end>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="thin">
-        <color rgb="FF000000"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="thin">
-        <color rgb="FF000000"/>
-      </end>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
@@ -387,7 +312,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -427,43 +352,25 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="10" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="11" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="13" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="11" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="5" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
@@ -518,7 +425,7 @@
       </c>
       <c r="B3">
         <f>Operators!B1</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3">
         <f>Operators!B2</f>
@@ -1115,17 +1022,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:F88"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" style="0" width="16.427584134615387" customWidth="1"/>
     <col min="3" max="5" style="0" width="9.142307692307693"/>
-    <col min="6" max="6" style="0" width="31.998076923076926" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" style="0" width="33.85510817307693" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
@@ -1135,7 +1042,7 @@
       </c>
       <c r="B1">
         <f t="array" ref="B1">SUM(0+E$24:E$9978)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
@@ -1724,10 +1631,8 @@
         <f>C66=D66</f>
         <v>1</v>
       </c>
-      <c r="F66" s="9" t="inlineStr">
-        <is>
-          <t>Regexp</t>
-        </is>
+      <c r="F66" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15">
@@ -1791,10 +1696,8 @@
       <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" ht="15">
-      <c r="A73" s="10" t="inlineStr">
-        <is>
-          <t>=string</t>
-        </is>
+      <c r="A73" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -1951,6 +1854,102 @@
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="12"/>
+    </row>
+    <row r="90" spans="1:6" ht="15">
+      <c r="A90" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8">
+        <f>DSUM($A$4:$B$19,"Value",A90:A91)</f>
+        <v>0</v>
+      </c>
+      <c r="D90" s="8">
+        <v>0</v>
+      </c>
+      <c r="E90" s="8" t="b">
+        <f>C90=D90</f>
+        <v>1</v>
+      </c>
+      <c r="F90" s="9"/>
+    </row>
+    <row r="91" spans="1:6" ht="15">
+      <c r="A91" s="10" t="inlineStr">
+        <is>
+          <t>=str</t>
+        </is>
+      </c>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="12"/>
+    </row>
+    <row r="93" spans="1:6" ht="15">
+      <c r="A93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8">
+        <f>DSUM($A$4:$B$19,"Value",A93:A94)</f>
+        <v>16384</v>
+      </c>
+      <c r="D93" s="8">
+        <v>16384</v>
+      </c>
+      <c r="E93" s="8" t="b">
+        <f>C93=D93</f>
+        <v>1</v>
+      </c>
+      <c r="F93" s="9" t="inlineStr">
+        <is>
+          <t>Regexp, not anchored at end</t>
+        </is>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15">
+      <c r="A94" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="12"/>
+    </row>
+    <row r="96" spans="1:6" ht="15">
+      <c r="A96" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8">
+        <f>DSUM($A$4:$B$19,"Value",A96:A97)</f>
+        <v>0</v>
+      </c>
+      <c r="D96" s="8">
+        <v>0</v>
+      </c>
+      <c r="E96" s="8" t="b">
+        <f>C96=D96</f>
+        <v>1</v>
+      </c>
+      <c r="F96" s="9" t="inlineStr">
+        <is>
+          <t>Regexp, anchorend at start</t>
+        </is>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15">
+      <c r="A97" s="10" t="inlineStr">
+        <is>
+          <t>ing</t>
+        </is>
+      </c>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="12"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2003,10 +2002,10 @@
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -2145,185 +2144,185 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15">
-      <c r="A20" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="15">
+      <c r="A20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8">
         <f>DSUM($A$4:$C$16,"Value",A20:B21)</f>
         <v>56</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="8">
         <v>56</v>
       </c>
-      <c r="E20" s="15" t="b">
+      <c r="E20" s="8" t="b">
         <f>C20=D20</f>
         <v>1</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>25</v>
+      <c r="F20" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="18" t="inlineStr">
+      <c r="B21" s="14" t="inlineStr">
         <is>
           <t>&lt;=6</t>
         </is>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="23" spans="1:6" ht="15">
-      <c r="A23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="15">
+      <c r="A23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="8">
         <f>DSUM($A$4:$C$16,"Value",A23:B24)</f>
         <v>4080</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="8">
         <v>4080</v>
       </c>
-      <c r="E23" s="15" t="b">
+      <c r="E23" s="8" t="b">
         <f>C23=D23</f>
         <v>1</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>25</v>
+      <c r="F23" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="18" t="inlineStr">
+      <c r="B24" s="14" t="inlineStr">
         <is>
           <t>&lt;=2</t>
         </is>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="26" spans="1:6" ht="15">
-      <c r="A26" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="15">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8">
         <f>DSUM($A$4:$C$16,"Value",A26:B27)</f>
         <v>192</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="8">
         <v>192</v>
       </c>
-      <c r="E26" s="15" t="b">
+      <c r="E26" s="8" t="b">
         <f>C26=D26</f>
         <v>1</v>
       </c>
-      <c r="F26" s="16" t="inlineStr">
+      <c r="F26" s="9" t="inlineStr">
         <is>
           <t>Conjunction</t>
         </is>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15">
-      <c r="A27" s="17" t="inlineStr">
+      <c r="A27" s="10" t="inlineStr">
         <is>
           <t>&gt;=7</t>
         </is>
       </c>
-      <c r="B27" s="18" t="inlineStr">
+      <c r="B27" s="14" t="inlineStr">
         <is>
           <t>&lt;=1</t>
         </is>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="29" spans="1:6" ht="15">
-      <c r="A29" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="15">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="8">
         <f>DSUM($A$4:$C$16,"Value",A29:A31)</f>
         <v>516</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="8">
         <v>516</v>
       </c>
-      <c r="E29" s="15" t="b">
+      <c r="E29" s="8" t="b">
         <f>C29=D29</f>
         <v>1</v>
       </c>
-      <c r="F29" s="16" t="inlineStr">
+      <c r="F29" s="9" t="inlineStr">
         <is>
           <t>Disjunction</t>
         </is>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15">
-      <c r="A30" s="22" t="inlineStr">
+      <c r="A30" s="16" t="inlineStr">
         <is>
           <t>=3</t>
         </is>
       </c>
-      <c r="B30" s="23"/>
-      <c r="F30" s="24"/>
+      <c r="B30" s="17"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="15">
-      <c r="A31" s="17" t="inlineStr">
+      <c r="A31" s="10" t="inlineStr">
         <is>
           <t>=10</t>
         </is>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="33" spans="1:6" ht="15">
-      <c r="A33" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="15">
+      <c r="A33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8">
         <f>DSUM($A$4:$C$16,"Value",A33:B35)</f>
         <v>960</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="8">
         <f>64+128+256+512</f>
         <v>960</v>
       </c>
-      <c r="E33" s="15" t="b">
+      <c r="E33" s="8" t="b">
         <f>C33=D33</f>
         <v>1</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15">
-      <c r="A34" s="22" t="inlineStr">
+      <c r="A34" s="16" t="inlineStr">
         <is>
           <t>&gt;6</t>
         </is>
@@ -2333,23 +2332,23 @@
           <t>=1</t>
         </is>
       </c>
-      <c r="F34" s="24"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" ht="15">
-      <c r="A35" s="17" t="inlineStr">
+      <c r="A35" s="10" t="inlineStr">
         <is>
           <t>&lt;11</t>
         </is>
       </c>
-      <c r="B35" s="18" t="inlineStr">
+      <c r="B35" s="14" t="inlineStr">
         <is>
           <t>=2</t>
         </is>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
D-funcs: fix problem with errors in the selector area.
We treated it as a zero while it should be treated as type incompatible.
</commit_message>
<xml_diff>
--- a/samples/excel12/database.xlsx
+++ b/samples/excel12/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="6230"/>
+    <workbookView activeTab="0" windowWidth="14400" windowHeight="7010"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="26">
   <si>
     <t>Types</t>
   </si>
@@ -98,15 +98,6 @@
   </si>
   <si>
     <t>Regexps only match strings</t>
-  </si>
-  <si>
-    <t>Regexp</t>
-  </si>
-  <si>
-    <t>=string</t>
-  </si>
-  <si>
-    <t>str</t>
   </si>
   <si>
     <t>Selector1</t>
@@ -1022,7 +1013,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <f t="array" ref="B1">SUM(0+E$24:E$9978)</f>
+        <f t="array" ref="B1">SUM(0+E$25:E$9979)</f>
         <v>25</v>
       </c>
     </row>
@@ -1050,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <f t="array" ref="B2">SUM(0+ISLOGICAL(E$24:E$9978))-B1</f>
+        <f t="array" ref="B2">SUM(0+ISLOGICAL(E$25:E$9979))-B1</f>
         <v>0</v>
       </c>
     </row>
@@ -1172,7 +1163,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
@@ -1180,776 +1171,790 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A24:A25)</f>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="6" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B20" s="6">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15">
+      <c r="A25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A25:A26)</f>
         <v>16</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="8">
         <v>16</v>
       </c>
-      <c r="E24" s="8" t="b">
-        <f>C24=D24</f>
-        <v>1</v>
-      </c>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" ht="15">
-      <c r="A25" s="10" t="inlineStr">
+      <c r="E25" s="8" t="b">
+        <f>C25=D25</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="15">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>=4</t>
         </is>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="27" spans="1:6" ht="15">
-      <c r="A27" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A27:A28)</f>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="28" spans="1:6" ht="15">
+      <c r="A28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A28:A29)</f>
         <v>15</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="8">
         <v>15</v>
       </c>
-      <c r="E27" s="8" t="b">
-        <f>C27=D27</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" ht="15">
-      <c r="A28" s="10" t="inlineStr">
+      <c r="E28" s="8" t="b">
+        <f>C28=D28</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="15">
+      <c r="A29" s="10" t="inlineStr">
         <is>
           <t>&lt;4</t>
         </is>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="30" spans="1:6" ht="15">
-      <c r="A30" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A30:A31)</f>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="15">
+      <c r="A31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A31:A32)</f>
         <v>2016</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="8">
         <v>2016</v>
       </c>
-      <c r="E30" s="8" t="b">
-        <f>C30=D30</f>
-        <v>1</v>
-      </c>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" ht="15">
-      <c r="A31" s="10" t="inlineStr">
+      <c r="E31" s="8" t="b">
+        <f>C31=D31</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="15">
+      <c r="A32" s="10" t="inlineStr">
         <is>
           <t>&gt;4</t>
         </is>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="33" spans="1:6" ht="15">
-      <c r="A33" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A33:A34)</f>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="34" spans="1:6" ht="15">
+      <c r="A34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A34:A35)</f>
         <v>31</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D34" s="8">
         <v>31</v>
       </c>
-      <c r="E33" s="8" t="b">
-        <f>C33=D33</f>
-        <v>1</v>
-      </c>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" ht="15">
-      <c r="A34" s="10" t="inlineStr">
+      <c r="E34" s="8" t="b">
+        <f>C34=D34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="15">
+      <c r="A35" s="10" t="inlineStr">
         <is>
           <t>&lt;=4</t>
         </is>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="36" spans="1:6" ht="15">
-      <c r="A36" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A36:A37)</f>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="37" spans="1:6" ht="15">
+      <c r="A37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A37:A38)</f>
         <v>2032</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <v>2032</v>
       </c>
-      <c r="E36" s="8" t="b">
-        <f>C36=D36</f>
-        <v>1</v>
-      </c>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" ht="15">
-      <c r="A37" s="10" t="s">
+      <c r="E37" s="8" t="b">
+        <f>C37=D37</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" ht="15">
+      <c r="A38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="39" spans="1:6" ht="15">
-      <c r="A39" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A39:A40)</f>
-        <v>32751</v>
-      </c>
-      <c r="D39" s="8">
-        <v>32751</v>
-      </c>
-      <c r="E39" s="8" t="b">
-        <f>C39=D39</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="9"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="40" spans="1:6" ht="15">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A40:A41)</f>
+        <v>65519</v>
+      </c>
+      <c r="D40" s="8">
+        <v>65519</v>
+      </c>
+      <c r="E40" s="8" t="b">
+        <f>C40=D40</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="15">
+      <c r="A41" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="42" spans="1:6" ht="15">
-      <c r="A42" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A42:A43)</f>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="43" spans="1:6" ht="15">
+      <c r="A43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A43:A44)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D43" s="8">
         <v>0</v>
       </c>
-      <c r="E42" s="8" t="b">
-        <f>C42=D42</f>
-        <v>1</v>
-      </c>
-      <c r="F42" s="9" t="s">
+      <c r="E43" s="8" t="b">
+        <f>C43=D43</f>
+        <v>1</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15">
-      <c r="A43" s="10" t="inlineStr">
+    <row r="44" spans="1:6" ht="15">
+      <c r="A44" s="10" t="inlineStr">
         <is>
           <t>1*</t>
         </is>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="45" spans="1:6" ht="15">
-      <c r="A45" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A45:A46)</f>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="46" spans="1:6" ht="15">
+      <c r="A46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A46:A47)</f>
         <v>16384</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D46" s="8">
         <v>16384</v>
       </c>
-      <c r="E45" s="8" t="b">
-        <f>C45=D45</f>
-        <v>1</v>
-      </c>
-      <c r="F45" s="9" t="s">
+      <c r="E46" s="8" t="b">
+        <f>C46=D46</f>
+        <v>1</v>
+      </c>
+      <c r="F46" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15">
-      <c r="A46" s="10" t="inlineStr">
+    <row r="47" spans="1:6" ht="15">
+      <c r="A47" s="10" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="12"/>
-    </row>
-    <row r="48" spans="1:6" ht="15">
-      <c r="A48" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A48:A49)</f>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="49" spans="1:6" ht="15">
+      <c r="A49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A49:A50)</f>
         <v>2048</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D49" s="8">
         <v>2048</v>
       </c>
-      <c r="E48" s="8" t="b">
-        <f>C48=D48</f>
-        <v>1</v>
-      </c>
-      <c r="F48" s="9" t="inlineStr">
+      <c r="E49" s="8" t="b">
+        <f>C49=D49</f>
+        <v>1</v>
+      </c>
+      <c r="F49" s="9" t="inlineStr">
         <is>
           <t>Blank (special case)</t>
         </is>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15">
-      <c r="A49" s="10" t="inlineStr">
+    <row r="50" spans="1:6" ht="15">
+      <c r="A50" s="10" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="51" spans="1:6" ht="15">
-      <c r="A51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A51:A52)</f>
-        <v>30719</v>
-      </c>
-      <c r="D51" s="8">
-        <f>2^15-1-2048</f>
-        <v>30719</v>
-      </c>
-      <c r="E51" s="8" t="b">
-        <f>C51=D51</f>
-        <v>1</v>
-      </c>
-      <c r="F51" s="9" t="inlineStr">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="52" spans="1:6" ht="15">
+      <c r="A52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A52:A53)</f>
+        <v>63487</v>
+      </c>
+      <c r="D52" s="8">
+        <v>63487</v>
+      </c>
+      <c r="E52" s="8" t="b">
+        <f>C52=D52</f>
+        <v>1</v>
+      </c>
+      <c r="F52" s="9" t="inlineStr">
         <is>
           <t>Non-blank (special case)</t>
         </is>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15">
-      <c r="A52" s="10" t="inlineStr">
+    <row r="53" spans="1:6" ht="15">
+      <c r="A53" s="10" t="inlineStr">
         <is>
           <t>&lt;&gt;</t>
         </is>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="54" spans="1:6" ht="15">
-      <c r="A54" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A54:A55)</f>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="55" spans="1:6" ht="15">
+      <c r="A55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A55:A56)</f>
         <v>64</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D55" s="8">
         <v>64</v>
       </c>
-      <c r="E54" s="8" t="b">
-        <f>C54=D54</f>
-        <v>1</v>
-      </c>
-      <c r="F54" s="9" t="inlineStr">
+      <c r="E55" s="8" t="b">
+        <f>C55=D55</f>
+        <v>1</v>
+      </c>
+      <c r="F55" s="9" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15">
-      <c r="A55" s="10">
+    <row r="56" spans="1:6" ht="15">
+      <c r="A56" s="10">
         <v>6</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="12"/>
-    </row>
-    <row r="57" spans="1:6" ht="15">
-      <c r="A57" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A57:A58)</f>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="58" spans="1:6" ht="15">
+      <c r="A58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A58:A59)</f>
         <v>8192</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D58" s="8">
         <v>8192</v>
       </c>
-      <c r="E57" s="8" t="b">
-        <f>C57=D57</f>
-        <v>1</v>
-      </c>
-      <c r="F57" s="9" t="s">
+      <c r="E58" s="8" t="b">
+        <f>C58=D58</f>
+        <v>1</v>
+      </c>
+      <c r="F58" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="12"/>
-    </row>
-    <row r="60" spans="1:6" ht="15">
-      <c r="A60" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A60:A61)</f>
+    <row r="59" spans="1:6">
+      <c r="A59" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="61" spans="1:6" ht="15">
+      <c r="A61" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A61:A62)</f>
         <v>4096</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D61" s="8">
         <v>4096</v>
       </c>
-      <c r="E60" s="8" t="b">
-        <f>C60=D60</f>
-        <v>1</v>
-      </c>
-      <c r="F60" s="9" t="s">
+      <c r="E61" s="8" t="b">
+        <f>C61=D61</f>
+        <v>1</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="10" t="b">
+    <row r="62" spans="1:6">
+      <c r="A62" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="63" spans="1:6" ht="15">
-      <c r="A63" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A63:A64)</f>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="64" spans="1:6" ht="15">
+      <c r="A64" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A64:A65)</f>
         <v>8192</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D64" s="8">
         <v>8192</v>
       </c>
-      <c r="E63" s="8" t="b">
-        <f>C63=D63</f>
-        <v>1</v>
-      </c>
-      <c r="F63" s="9" t="inlineStr">
+      <c r="E64" s="8" t="b">
+        <f>C64=D64</f>
+        <v>1</v>
+      </c>
+      <c r="F64" s="9" t="inlineStr">
         <is>
           <t>Boolean as string</t>
         </is>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15">
-      <c r="A64" s="10" t="inlineStr">
+    <row r="65" spans="1:6" ht="15">
+      <c r="A65" s="10" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="66" spans="1:6" ht="15">
-      <c r="A66" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A66:A67)</f>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="67" spans="1:6" ht="15">
+      <c r="A67" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A67:A68)</f>
         <v>16384</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D67" s="8">
         <v>16384</v>
       </c>
-      <c r="E66" s="8" t="b">
-        <f>C66=D66</f>
-        <v>1</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15">
-      <c r="A67" s="10" t="s">
+      <c r="E67" s="8" t="b">
+        <f>C67=D67</f>
+        <v>1</v>
+      </c>
+      <c r="F67" s="9" t="inlineStr">
+        <is>
+          <t>Regexp</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15">
+      <c r="A68" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="12"/>
-    </row>
-    <row r="69" spans="1:6" ht="15">
-      <c r="A69" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A69:A70)</f>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="70" spans="1:6" ht="15">
+      <c r="A70" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A70:A71)</f>
         <v>16384</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D70" s="8">
         <v>16384</v>
       </c>
-      <c r="E69" s="8" t="b">
-        <f>C69=D69</f>
-        <v>1</v>
-      </c>
-      <c r="F69" s="9" t="inlineStr">
+      <c r="E70" s="8" t="b">
+        <f>C70=D70</f>
+        <v>1</v>
+      </c>
+      <c r="F70" s="9" t="inlineStr">
         <is>
           <t>Regexp, different case</t>
         </is>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15">
-      <c r="A70" s="10" t="s">
+    <row r="71" spans="1:6" ht="15">
+      <c r="A71" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="12"/>
-    </row>
-    <row r="72" spans="1:6" ht="15">
-      <c r="A72" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A72:A73)</f>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="73" spans="1:6" ht="15">
+      <c r="A73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A73:A74)</f>
         <v>16384</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D73" s="8">
         <v>16384</v>
       </c>
-      <c r="E72" s="8" t="b">
-        <f>C72=D72</f>
-        <v>1</v>
-      </c>
-      <c r="F72" s="9"/>
-    </row>
-    <row r="73" spans="1:6" ht="15">
-      <c r="A73" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="12"/>
-    </row>
-    <row r="75" spans="1:6" ht="15">
-      <c r="A75" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A75:A76)</f>
+      <c r="E73" s="8" t="b">
+        <f>C73=D73</f>
+        <v>1</v>
+      </c>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="1:6" ht="15">
+      <c r="A74" s="10" t="inlineStr">
+        <is>
+          <t>=string</t>
+        </is>
+      </c>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="12"/>
+    </row>
+    <row r="76" spans="1:6" ht="15">
+      <c r="A76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A76:A77)</f>
         <v>0</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D76" s="8">
         <v>0</v>
       </c>
-      <c r="E75" s="8" t="b">
-        <f>C75=D75</f>
-        <v>1</v>
-      </c>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" ht="15">
-      <c r="A76" s="10" t="inlineStr">
+      <c r="E76" s="8" t="b">
+        <f>C76=D76</f>
+        <v>1</v>
+      </c>
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" ht="15">
+      <c r="A77" s="10" t="inlineStr">
         <is>
           <t>&lt;string</t>
         </is>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="12"/>
-    </row>
-    <row r="78" spans="1:6" ht="15">
-      <c r="A78" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A78:A79)</f>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="79" spans="1:6" ht="15">
+      <c r="A79" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A79:A80)</f>
         <v>0</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D79" s="8">
         <v>0</v>
       </c>
-      <c r="E78" s="8" t="b">
-        <f>C78=D78</f>
-        <v>1</v>
-      </c>
-      <c r="F78" s="9"/>
-    </row>
-    <row r="79" spans="1:6" ht="15">
-      <c r="A79" s="10" t="inlineStr">
+      <c r="E79" s="8" t="b">
+        <f>C79=D79</f>
+        <v>1</v>
+      </c>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80" spans="1:6" ht="15">
+      <c r="A80" s="10" t="inlineStr">
         <is>
           <t>&gt;string</t>
         </is>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="12"/>
-    </row>
-    <row r="81" spans="1:6" ht="15">
-      <c r="A81" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A81:A82)</f>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="82" spans="1:6" ht="15">
+      <c r="A82" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A82:A83)</f>
         <v>16384</v>
       </c>
-      <c r="D81" s="8">
+      <c r="D82" s="8">
         <v>16384</v>
       </c>
-      <c r="E81" s="8" t="b">
-        <f>C81=D81</f>
-        <v>1</v>
-      </c>
-      <c r="F81" s="9"/>
-    </row>
-    <row r="82" spans="1:6" ht="15">
-      <c r="A82" s="10" t="inlineStr">
+      <c r="E82" s="8" t="b">
+        <f>C82=D82</f>
+        <v>1</v>
+      </c>
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="1:6" ht="15">
+      <c r="A83" s="10" t="inlineStr">
         <is>
           <t>&lt;=string</t>
         </is>
       </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="12"/>
-    </row>
-    <row r="84" spans="1:6" ht="15">
-      <c r="A84" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A84:A85)</f>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="85" spans="1:6" ht="15">
+      <c r="A85" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A85:A86)</f>
         <v>16384</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D85" s="8">
         <v>16384</v>
       </c>
-      <c r="E84" s="8" t="b">
-        <f>C84=D84</f>
-        <v>1</v>
-      </c>
-      <c r="F84" s="9"/>
-    </row>
-    <row r="85" spans="1:6" ht="15">
-      <c r="A85" s="10" t="inlineStr">
+      <c r="E85" s="8" t="b">
+        <f>C85=D85</f>
+        <v>1</v>
+      </c>
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="1:6" ht="15">
+      <c r="A86" s="10" t="inlineStr">
         <is>
           <t>&gt;=string</t>
         </is>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="12"/>
-    </row>
-    <row r="87" spans="1:6" ht="15">
-      <c r="A87" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A87:A88)</f>
-        <v>16383</v>
-      </c>
-      <c r="D87" s="8">
-        <v>16383</v>
-      </c>
-      <c r="E87" s="8" t="b">
-        <f>C87=D87</f>
-        <v>1</v>
-      </c>
-      <c r="F87" s="9"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="12"/>
     </row>
     <row r="88" spans="1:6" ht="15">
-      <c r="A88" s="10" t="inlineStr">
+      <c r="A88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A88:A89)</f>
+        <v>49151</v>
+      </c>
+      <c r="D88" s="8">
+        <v>49151</v>
+      </c>
+      <c r="E88" s="8" t="b">
+        <f>C88=D88</f>
+        <v>1</v>
+      </c>
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="1:6" ht="15">
+      <c r="A89" s="10" t="inlineStr">
         <is>
           <t>&lt;&gt;string</t>
         </is>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="90" spans="1:6" ht="15">
-      <c r="A90" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A90:A91)</f>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="12"/>
+    </row>
+    <row r="91" spans="1:6" ht="15">
+      <c r="A91" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A91:A92)</f>
         <v>0</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D91" s="8">
         <v>0</v>
       </c>
-      <c r="E90" s="8" t="b">
-        <f>C90=D90</f>
-        <v>1</v>
-      </c>
-      <c r="F90" s="9"/>
-    </row>
-    <row r="91" spans="1:6" ht="15">
-      <c r="A91" s="10" t="inlineStr">
+      <c r="E91" s="8" t="b">
+        <f>C91=D91</f>
+        <v>1</v>
+      </c>
+      <c r="F91" s="9"/>
+    </row>
+    <row r="92" spans="1:6" ht="15">
+      <c r="A92" s="10" t="inlineStr">
         <is>
           <t>=str</t>
         </is>
       </c>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="12"/>
-    </row>
-    <row r="93" spans="1:6" ht="15">
-      <c r="A93" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A93:A94)</f>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="12"/>
+    </row>
+    <row r="94" spans="1:6" ht="15">
+      <c r="A94" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A94:A95)</f>
         <v>16384</v>
       </c>
-      <c r="D93" s="8">
+      <c r="D94" s="8">
         <v>16384</v>
       </c>
-      <c r="E93" s="8" t="b">
-        <f>C93=D93</f>
-        <v>1</v>
-      </c>
-      <c r="F93" s="9" t="inlineStr">
+      <c r="E94" s="8" t="b">
+        <f>C94=D94</f>
+        <v>1</v>
+      </c>
+      <c r="F94" s="9" t="inlineStr">
         <is>
           <t>Regexp, not anchored at end</t>
         </is>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15">
-      <c r="A94" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="12"/>
-    </row>
-    <row r="96" spans="1:6" ht="15">
-      <c r="A96" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8">
-        <f>DSUM($A$4:$B$19,"Value",A96:A97)</f>
+    <row r="95" spans="1:6" ht="15">
+      <c r="A95" s="10" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="12"/>
+    </row>
+    <row r="97" spans="1:6" ht="15">
+      <c r="A97" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8">
+        <f>DSUM($A$4:$B$20,"Value",A97:A98)</f>
         <v>0</v>
       </c>
-      <c r="D96" s="8">
+      <c r="D97" s="8">
         <v>0</v>
       </c>
-      <c r="E96" s="8" t="b">
-        <f>C96=D96</f>
-        <v>1</v>
-      </c>
-      <c r="F96" s="9" t="inlineStr">
+      <c r="E97" s="8" t="b">
+        <f>C97=D97</f>
+        <v>1</v>
+      </c>
+      <c r="F97" s="9" t="inlineStr">
         <is>
           <t>Regexp, anchorend at start</t>
         </is>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15">
-      <c r="A97" s="10" t="inlineStr">
+    <row r="98" spans="1:6" ht="15">
+      <c r="A98" s="10" t="inlineStr">
         <is>
           <t>ing</t>
         </is>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="12"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2002,10 +2007,10 @@
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -2145,10 +2150,10 @@
     </row>
     <row r="20" spans="1:6" ht="15">
       <c r="A20" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" s="8">
         <f>DSUM($A$4:$C$16,"Value",A20:B21)</f>
@@ -2162,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15">
@@ -2181,10 +2186,10 @@
     </row>
     <row r="23" spans="1:6" ht="15">
       <c r="A23" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" s="8">
         <f>DSUM($A$4:$C$16,"Value",A23:B24)</f>
@@ -2198,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15">
@@ -2217,10 +2222,10 @@
     </row>
     <row r="26" spans="1:6" ht="15">
       <c r="A26" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C26" s="8">
         <f>DSUM($A$4:$C$16,"Value",A26:B27)</f>
@@ -2257,7 +2262,7 @@
     </row>
     <row r="29" spans="1:6" ht="15">
       <c r="A29" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="8">
@@ -2300,10 +2305,10 @@
     </row>
     <row r="33" spans="1:6" ht="15">
       <c r="A33" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33" s="8">
         <f>DSUM($A$4:$C$16,"Value",A33:B35)</f>

</xml_diff>